<commit_message>
Updated sample country exchange rate in IHT database.
</commit_message>
<xml_diff>
--- a/SourceData/ohtcore/IHModData.xlsx
+++ b/SourceData/ohtcore/IHModData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\ohtcore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29E2606-C965-490F-B05F-84F45B79FD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BB7AC3-85C2-474F-9241-713977DF90DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CommentsOutline" sheetId="2" r:id="rId1"/>
@@ -6290,8 +6290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H464"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30630,8 +30630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D8DDA6-9117-4ADB-B296-670BDA511577}">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32853,7 +32853,7 @@
         <v>1966</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added default inflation values to exchange rate database.
</commit_message>
<xml_diff>
--- a/SourceData/ohtcore/IHModData.xlsx
+++ b/SourceData/ohtcore/IHModData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\ohtcore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BB7AC3-85C2-474F-9241-713977DF90DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF13D078-470C-4B7E-B331-99041193B3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,28 @@
     <sheet name="Tags" sheetId="4" r:id="rId3"/>
     <sheet name="ExchangeRateDB" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="1968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3258" uniqueCount="1971">
   <si>
     <t>Intervention Coverages</t>
   </si>
@@ -5922,9 +5933,6 @@
     <t>ZWE</t>
   </si>
   <si>
-    <t>&lt;Data&gt;</t>
-  </si>
-  <si>
     <t>&lt;ISO Alpha-3 Country Code&gt;</t>
   </si>
   <si>
@@ -5932,6 +5940,18 @@
   </si>
   <si>
     <t>CHA</t>
+  </si>
+  <si>
+    <t>&lt;Inflation Rate&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Inflation Rate Source&gt;</t>
+  </si>
+  <si>
+    <t>World Development Indicators</t>
+  </si>
+  <si>
+    <t>&lt;Inflation Rate Last Update&gt;</t>
   </si>
 </sst>
 </file>
@@ -5941,12 +5961,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5967,18 +5993,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{7E262D65-9DFC-4FE9-9672-D6D67E4FBFAB}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -30628,15 +30678,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D8DDA6-9117-4ADB-B296-670BDA511577}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="I151" sqref="I151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1747</v>
       </c>
@@ -30644,21 +30698,33 @@
         <v>152</v>
       </c>
       <c r="C1" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="D1" t="s">
-        <v>1964</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1452</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1967</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1968</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1748</v>
       </c>
       <c r="D2">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2022</v>
+      </c>
+      <c r="E2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -30669,10 +30735,19 @@
         <v>1749</v>
       </c>
       <c r="D3">
-        <v>76.813536435489695</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88.5</v>
+      </c>
+      <c r="E3">
+        <v>2.30237251516819</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G3" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -30683,10 +30758,19 @@
         <v>1750</v>
       </c>
       <c r="D4">
-        <v>103.52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>113.041667</v>
+      </c>
+      <c r="E4">
+        <v>6.7252027153004903</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>12</v>
       </c>
@@ -30697,10 +30781,19 @@
         <v>1751</v>
       </c>
       <c r="D5">
-        <v>135.06405833333301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>141.99497500000001</v>
+      </c>
+      <c r="E5">
+        <v>9.2655155155155295</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>24</v>
       </c>
@@ -30711,10 +30804,19 @@
         <v>1752</v>
       </c>
       <c r="D6">
-        <v>631.44195550672703</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>499.84791666669997</v>
+      </c>
+      <c r="E6">
+        <v>25.7542656453085</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G6" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>28</v>
       </c>
@@ -30727,8 +30829,17 @@
       <c r="D7">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>7.5310783463428903</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G7" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>32</v>
       </c>
@@ -30739,10 +30850,19 @@
         <v>1754</v>
       </c>
       <c r="D8">
-        <v>94.990741666666693</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130.6165</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G8" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>51</v>
       </c>
@@ -30753,10 +30873,19 @@
         <v>1755</v>
       </c>
       <c r="D9">
-        <v>503.76967496165202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>435.67</v>
+      </c>
+      <c r="E9">
+        <v>8.6409110897385499</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G9" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>533</v>
       </c>
@@ -30769,8 +30898,17 @@
       <c r="D10">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>4.2574620433542796</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G10" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>36</v>
       </c>
@@ -30781,10 +30919,19 @@
         <v>1757</v>
       </c>
       <c r="D11">
-        <v>1.3312242595708099</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.378193</v>
+      </c>
+      <c r="E11">
+        <v>6.5940967134184598</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G11" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>40</v>
       </c>
@@ -30795,10 +30942,19 @@
         <v>1758</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E12">
+        <v>8.5468699318844994</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G12" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>31</v>
       </c>
@@ -30811,8 +30967,17 @@
       <c r="D13">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>13.8522590144267</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G13" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>44</v>
       </c>
@@ -30825,8 +30990,17 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>5.6054063358304402</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G14" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>48</v>
       </c>
@@ -30839,8 +31013,17 @@
       <c r="D15">
         <v>0.376</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>3.6257410430448198</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G15" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>50</v>
       </c>
@@ -30851,10 +31034,19 @@
         <v>1762</v>
       </c>
       <c r="D16">
-        <v>85.083763250000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>86.303899999999999</v>
+      </c>
+      <c r="E16">
+        <v>7.6969543717685802</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G16" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>52</v>
       </c>
@@ -30867,8 +31059,17 @@
       <c r="D17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>4.1002896451846098</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G17" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>112</v>
       </c>
@@ -30879,10 +31080,19 @@
         <v>1764</v>
       </c>
       <c r="D18">
-        <v>2.538675</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.629</v>
+      </c>
+      <c r="E18">
+        <v>15.209675274080899</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G18" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>56</v>
       </c>
@@ -30893,10 +31103,19 @@
         <v>1765</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E19">
+        <v>9.5975117287249994</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G19" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>84</v>
       </c>
@@ -30909,8 +31128,17 @@
       <c r="D20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>6.2768931944754396</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G20" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>204</v>
       </c>
@@ -30921,10 +31149,19 @@
         <v>1767</v>
       </c>
       <c r="D21">
-        <v>554.602599205008</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.93731193229996</v>
+      </c>
+      <c r="E21">
+        <v>1.3507786358357099</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G21" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>64</v>
       </c>
@@ -30935,10 +31172,19 @@
         <v>1768</v>
       </c>
       <c r="D22">
-        <v>73.939348249405796</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>78.597570000000005</v>
+      </c>
+      <c r="E22">
+        <v>5.6391667139636503</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G22" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>68</v>
       </c>
@@ -30951,8 +31197,17 @@
       <c r="D23">
         <v>6.91</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1.7463287294596901</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G23" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>70</v>
       </c>
@@ -30963,10 +31218,19 @@
         <v>1770</v>
       </c>
       <c r="D24">
-        <v>1.65360615435868</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.859326</v>
+      </c>
+      <c r="E24">
+        <v>2.0526745200172698</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G24" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>72</v>
       </c>
@@ -30977,10 +31241,19 @@
         <v>1771</v>
       </c>
       <c r="D25">
-        <v>11.087258333333301</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12.368808333300001</v>
+      </c>
+      <c r="E25">
+        <v>11.665567478802</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G25" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>76</v>
       </c>
@@ -30991,10 +31264,19 @@
         <v>1772</v>
       </c>
       <c r="D26">
-        <v>5.3944007896250303</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5.1639699999999999</v>
+      </c>
+      <c r="E26">
+        <v>9.2801060895687293</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G26" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>96</v>
       </c>
@@ -31005,10 +31287,19 @@
         <v>1773</v>
       </c>
       <c r="D27">
-        <v>1.34380696297339</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3789560000000001</v>
+      </c>
+      <c r="E27">
+        <v>3.6822503060421599</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G27" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>100</v>
       </c>
@@ -31019,10 +31310,19 @@
         <v>1774</v>
       </c>
       <c r="D28">
-        <v>1.653775</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.8573999999999999</v>
+      </c>
+      <c r="E28">
+        <v>15.3252589264366</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G28" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>854</v>
       </c>
@@ -31033,10 +31333,19 @@
         <v>1775</v>
       </c>
       <c r="D29">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E29">
+        <v>14.2902354303358</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G29" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>108</v>
       </c>
@@ -31047,10 +31356,19 @@
         <v>1776</v>
       </c>
       <c r="D30">
-        <v>1975.9508813876801</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2387.05537</v>
+      </c>
+      <c r="E30">
+        <v>18.800878666494501</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G30" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>116</v>
       </c>
@@ -31061,10 +31379,19 @@
         <v>1777</v>
       </c>
       <c r="D31">
-        <v>4098.7227950588904</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4102.0378650000002</v>
+      </c>
+      <c r="E31">
+        <v>5.3437026489543697</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G31" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>120</v>
       </c>
@@ -31075,10 +31402,19 @@
         <v>1778</v>
       </c>
       <c r="D32">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E32">
+        <v>6.2476771334387902</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G32" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>124</v>
       </c>
@@ -31089,10 +31425,19 @@
         <v>1779</v>
       </c>
       <c r="D33">
-        <v>1.2538769021267999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3015547747435501</v>
+      </c>
+      <c r="E33">
+        <v>6.8028011534161301</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G33" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>132</v>
       </c>
@@ -31103,10 +31448,19 @@
         <v>1780</v>
       </c>
       <c r="D34">
-        <v>93.218092411610897</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>105.5308</v>
+      </c>
+      <c r="E34">
+        <v>7.93092925430087</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G34" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>140</v>
       </c>
@@ -31117,10 +31471,19 @@
         <v>1781</v>
       </c>
       <c r="D35">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E35">
+        <v>5.5831673518324703</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G35" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>148</v>
       </c>
@@ -31131,10 +31494,19 @@
         <v>1782</v>
       </c>
       <c r="D36">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E36">
+        <v>5.7880268784361597</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G36" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>830</v>
       </c>
@@ -31142,13 +31514,22 @@
         <v>1783</v>
       </c>
       <c r="C37" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G37" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>152</v>
       </c>
@@ -31159,10 +31540,19 @@
         <v>1784</v>
       </c>
       <c r="D38">
-        <v>758.955378658977</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>872.33151999999995</v>
+      </c>
+      <c r="E38">
+        <v>11.6438667110561</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G38" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>156</v>
       </c>
@@ -31173,10 +31563,19 @@
         <v>1785</v>
       </c>
       <c r="D39">
-        <v>6.4489751802431599</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.737158</v>
+      </c>
+      <c r="E39">
+        <v>1.97357555739051</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G39" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>344</v>
       </c>
@@ -31189,8 +31588,17 @@
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>1.88136707196912</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G40" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>446</v>
       </c>
@@ -31201,10 +31609,19 @@
         <v>1788</v>
       </c>
       <c r="D41">
-        <v>8.0055317499999994</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.0652059999999999</v>
+      </c>
+      <c r="E41">
+        <v>1.0450280236998799</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G41" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>158</v>
       </c>
@@ -31217,8 +31634,17 @@
       <c r="D42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G42" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>170</v>
       </c>
@@ -31229,10 +31655,19 @@
         <v>1792</v>
       </c>
       <c r="D43">
-        <v>3743.5898191968699</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4256.1941666666999</v>
+      </c>
+      <c r="E43">
+        <v>10.1772313546166</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G43" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>174</v>
       </c>
@@ -31243,10 +31678,19 @@
         <v>1793</v>
       </c>
       <c r="D44">
-        <v>415.95584914812201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>467.18426118719998</v>
+      </c>
+      <c r="E44">
+        <v>6.3147445031519602</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G44" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>178</v>
       </c>
@@ -31257,10 +31701,19 @@
         <v>1794</v>
       </c>
       <c r="D45">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.76002000000005</v>
+      </c>
+      <c r="E45">
+        <v>3.0434433469847799</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G45" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>188</v>
       </c>
@@ -31271,10 +31724,19 @@
         <v>1795</v>
       </c>
       <c r="D46">
-        <v>620.78472001408102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>647.13581799999997</v>
+      </c>
+      <c r="E46">
+        <v>8.2747749023265396</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G46" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>384</v>
       </c>
@@ -31285,10 +31747,19 @@
         <v>1796</v>
       </c>
       <c r="D47">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970090999999</v>
+      </c>
+      <c r="E47">
+        <v>5.2761672426284596</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G47" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>191</v>
       </c>
@@ -31299,10 +31770,19 @@
         <v>1797</v>
       </c>
       <c r="D48">
-        <v>6.3600831666666702</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375320000003</v>
+      </c>
+      <c r="E48">
+        <v>10.780580675868601</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G48" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>192</v>
       </c>
@@ -31313,10 +31793,19 @@
         <v>1798</v>
       </c>
       <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G49" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>531</v>
       </c>
@@ -31329,8 +31818,17 @@
       <c r="D50">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>2.6222078342505899</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G50" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>196</v>
       </c>
@@ -31341,10 +31839,19 @@
         <v>1800</v>
       </c>
       <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962400000000002</v>
+      </c>
+      <c r="E51">
+        <v>8.39548297993373</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G51" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>203</v>
       </c>
@@ -31355,10 +31862,19 @@
         <v>1801</v>
       </c>
       <c r="D52">
-        <v>21.678166666666701</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23.356999999999999</v>
+      </c>
+      <c r="E52">
+        <v>15.100165146837099</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G52" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>408</v>
       </c>
@@ -31369,10 +31885,19 @@
         <v>1802</v>
       </c>
       <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G53" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>180</v>
       </c>
@@ -31383,10 +31908,19 @@
         <v>1803</v>
       </c>
       <c r="D54">
-        <v>1989.3914712282799</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2009.8</v>
+      </c>
+      <c r="E54">
+        <v>2.8858510728998801</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G54" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>208</v>
       </c>
@@ -31397,10 +31931,19 @@
         <v>1804</v>
       </c>
       <c r="D55">
-        <v>6.2871130825000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.0761518624999997</v>
+      </c>
+      <c r="E55">
+        <v>7.6965669988926004</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G55" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>262</v>
       </c>
@@ -31413,8 +31956,17 @@
       <c r="D56">
         <v>177.721</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>5.1798084796707098</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G56" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>212</v>
       </c>
@@ -31427,8 +31979,17 @@
       <c r="D57">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>1.50462353858112</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G57" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>214</v>
       </c>
@@ -31439,10 +32000,19 @@
         <v>1807</v>
       </c>
       <c r="D58">
-        <v>57.221116666666703</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55.140999999999998</v>
+      </c>
+      <c r="E58">
+        <v>8.8110920927958691</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G58" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>218</v>
       </c>
@@ -31455,8 +32025,17 @@
       <c r="D59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>3.4661697221307701</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G59" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>818</v>
       </c>
@@ -31467,10 +32046,19 @@
         <v>1809</v>
       </c>
       <c r="D60">
-        <v>15.644527277711299</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.45</v>
+      </c>
+      <c r="E60">
+        <v>13.895660977517799</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G60" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>222</v>
       </c>
@@ -31483,8 +32071,17 @@
       <c r="D61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>7.1986161560979101</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G61" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>226</v>
       </c>
@@ -31495,10 +32092,19 @@
         <v>1811</v>
       </c>
       <c r="D62">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970091119996</v>
+      </c>
+      <c r="E62">
+        <v>4.7867170471080298</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G62" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>232</v>
       </c>
@@ -31511,8 +32117,17 @@
       <c r="D63">
         <v>15.074999999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G63" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>233</v>
       </c>
@@ -31523,10 +32138,19 @@
         <v>1813</v>
       </c>
       <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E64">
+        <v>19.398263408061599</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G64" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>231</v>
       </c>
@@ -31537,10 +32161,19 @@
         <v>1814</v>
       </c>
       <c r="D65">
-        <v>34.927165404040402</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48.567355999999997</v>
+      </c>
+      <c r="E65">
+        <v>33.889879710089801</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G65" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>242</v>
       </c>
@@ -31551,10 +32184,19 @@
         <v>1815</v>
       </c>
       <c r="D66">
-        <v>2.0706333333333302</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.2014070000000001</v>
+      </c>
+      <c r="E66">
+        <v>4.5201926639495804</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G66" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>246</v>
       </c>
@@ -31565,10 +32207,19 @@
         <v>1816</v>
       </c>
       <c r="D67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E67">
+        <v>7.1235077330140202</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G67" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>250</v>
       </c>
@@ -31579,10 +32230,19 @@
         <v>1817</v>
       </c>
       <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E68">
+        <v>5.2223674836973499</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G68" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>254</v>
       </c>
@@ -31595,8 +32255,17 @@
       <c r="D69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G69" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>258</v>
       </c>
@@ -31607,10 +32276,19 @@
         <v>1820</v>
       </c>
       <c r="D70">
-        <v>100.88022256618601</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+        <v>113.474367</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G70" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>266</v>
       </c>
@@ -31621,10 +32299,19 @@
         <v>1821</v>
       </c>
       <c r="D71">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E71">
+        <v>4.23124798274619</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G71" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>270</v>
       </c>
@@ -31635,10 +32322,19 @@
         <v>1822</v>
       </c>
       <c r="D72">
-        <v>51.484443878383303</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55.276666666700002</v>
+      </c>
+      <c r="E72">
+        <v>11.513119838050599</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G72" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>268</v>
       </c>
@@ -31649,10 +32345,19 @@
         <v>1823</v>
       </c>
       <c r="D73">
-        <v>3.2215583333333302</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.9161999999999999</v>
+      </c>
+      <c r="E73">
+        <v>11.898165420319801</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G73" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>276</v>
       </c>
@@ -31663,10 +32368,19 @@
         <v>1824</v>
       </c>
       <c r="D74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E74">
+        <v>6.87257438551097</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G74" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>288</v>
       </c>
@@ -31677,10 +32391,19 @@
         <v>1825</v>
       </c>
       <c r="D75">
-        <v>5.8056999999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.2723999999999993</v>
+      </c>
+      <c r="E75">
+        <v>31.255895104901601</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G75" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>300</v>
       </c>
@@ -31691,10 +32414,19 @@
         <v>1826</v>
       </c>
       <c r="D76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E76">
+        <v>9.6452598128063194</v>
+      </c>
+      <c r="F76" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G76" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>308</v>
       </c>
@@ -31707,8 +32439,17 @@
       <c r="D77">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E77">
+        <v>2.5597891192934199</v>
+      </c>
+      <c r="F77" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G77" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>312</v>
       </c>
@@ -31721,8 +32462,17 @@
       <c r="D78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G78" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>316</v>
       </c>
@@ -31735,8 +32485,17 @@
       <c r="D79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G79" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>320</v>
       </c>
@@ -31747,10 +32506,19 @@
         <v>1831</v>
       </c>
       <c r="D80">
-        <v>7.7343883333333299</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7.7482439999999997</v>
+      </c>
+      <c r="E80">
+        <v>6.8851282334428703</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G80" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>324</v>
       </c>
@@ -31761,10 +32529,19 @@
         <v>1832</v>
       </c>
       <c r="D81">
-        <v>9565.0821834383296</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8694.1003999999994</v>
+      </c>
+      <c r="E81">
+        <v>10.4930409984424</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G81" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>624</v>
       </c>
@@ -31775,10 +32552,19 @@
         <v>1833</v>
       </c>
       <c r="D82">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970090999999</v>
+      </c>
+      <c r="E82">
+        <v>9.3938387745652694</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G82" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>328</v>
       </c>
@@ -31791,8 +32577,17 @@
       <c r="D83">
         <v>208.5</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E83">
+        <v>6.1150555010993504</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G83" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>332</v>
       </c>
@@ -31803,10 +32598,19 @@
         <v>1835</v>
       </c>
       <c r="D84">
-        <v>89.226636511630403</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107.05395719000001</v>
+      </c>
+      <c r="E84">
+        <v>33.983931947069998</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G84" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>340</v>
       </c>
@@ -31817,10 +32621,19 @@
         <v>1836</v>
       </c>
       <c r="D85">
-        <v>24.0166553242681</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>24.485873999999999</v>
+      </c>
+      <c r="E85">
+        <v>9.0896391152502503</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G85" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>348</v>
       </c>
@@ -31831,10 +32644,19 @@
         <v>1837</v>
       </c>
       <c r="D86">
-        <v>303.14083333333298</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>372.59583333333302</v>
+      </c>
+      <c r="E86">
+        <v>14.608143949243299</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G86" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>352</v>
       </c>
@@ -31845,10 +32667,19 @@
         <v>1838</v>
       </c>
       <c r="D87">
-        <v>126.988860204557</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>135.27990200138001</v>
+      </c>
+      <c r="E87">
+        <v>8.3087551155892001</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G87" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>356</v>
       </c>
@@ -31859,10 +32690,19 @@
         <v>1839</v>
       </c>
       <c r="D88">
-        <v>73.918012815435105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79.729399999999998</v>
+      </c>
+      <c r="E88">
+        <v>6.6990341407983003</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G88" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>360</v>
       </c>
@@ -31873,10 +32713,19 @@
         <v>1840</v>
       </c>
       <c r="D89">
-        <v>14308.1439011897</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14849.853936</v>
+      </c>
+      <c r="E89">
+        <v>4.2094638340216504</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G89" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>364</v>
       </c>
@@ -31887,10 +32736,19 @@
         <v>1841</v>
       </c>
       <c r="D90">
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <v>252362.18660136699</v>
+      </c>
+      <c r="E90">
+        <v>43.488464174217903</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G90" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>368</v>
       </c>
@@ -31903,8 +32761,17 @@
       <c r="D91">
         <v>1450</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E91">
+        <v>4.9947659638104396</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G91" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>372</v>
       </c>
@@ -31915,10 +32782,19 @@
         <v>1843</v>
       </c>
       <c r="D92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E92">
+        <v>7.8073754099671602</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G92" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>376</v>
       </c>
@@ -31929,10 +32805,19 @@
         <v>1844</v>
       </c>
       <c r="D93">
-        <v>3.23019832251082</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.3596144015818901</v>
+      </c>
+      <c r="E93">
+        <v>4.3935966591265396</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G93" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>380</v>
       </c>
@@ -31943,10 +32828,19 @@
         <v>1845</v>
       </c>
       <c r="D94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E94">
+        <v>8.2012899116171791</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G94" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>388</v>
       </c>
@@ -31957,10 +32851,19 @@
         <v>1846</v>
       </c>
       <c r="D95">
-        <v>142.402832756013</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+        <v>153.42681666670001</v>
+      </c>
+      <c r="E95">
+        <v>10.3495688391274</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G95" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>392</v>
       </c>
@@ -31971,10 +32874,19 @@
         <v>1847</v>
       </c>
       <c r="D96">
-        <v>109.754323839417</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+        <v>131.49814044376399</v>
+      </c>
+      <c r="E96">
+        <v>2.4977027817225501</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G96" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>400</v>
       </c>
@@ -31987,8 +32899,17 @@
       <c r="D97">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E97">
+        <v>4.2291556889711703</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G97" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>398</v>
       </c>
@@ -31999,10 +32920,19 @@
         <v>1849</v>
       </c>
       <c r="D98">
-        <v>425.90750000000003</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <v>460.16500000000002</v>
+      </c>
+      <c r="E98">
+        <v>8.0423206278027592</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G98" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>404</v>
       </c>
@@ -32013,10 +32943,19 @@
         <v>1850</v>
       </c>
       <c r="D99">
-        <v>109.63774659236699</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+        <v>117.86579999999999</v>
+      </c>
+      <c r="E99">
+        <v>7.65687456104604</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G99" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>296</v>
       </c>
@@ -32027,10 +32966,19 @@
         <v>1851</v>
       </c>
       <c r="D100">
-        <v>1.3312242595708099</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.4416640000000001</v>
+      </c>
+      <c r="E100">
+        <v>2.05361676773907</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G100" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>414</v>
       </c>
@@ -32041,10 +32989,19 @@
         <v>1852</v>
       </c>
       <c r="D101">
-        <v>0.30164311076994899</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.30625000000000002</v>
+      </c>
+      <c r="E101">
+        <v>3.9806496199031298</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G101" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>417</v>
       </c>
@@ -32055,10 +33012,19 @@
         <v>1853</v>
       </c>
       <c r="D102">
-        <v>84.640822006528495</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84.116225999999997</v>
+      </c>
+      <c r="E102">
+        <v>13.922909317417499</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G102" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>418</v>
       </c>
@@ -32069,10 +33035,19 @@
         <v>1854</v>
       </c>
       <c r="D103">
-        <v>9697.91578947368</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14035.226693000001</v>
+      </c>
+      <c r="E103">
+        <v>22.956222513205599</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G103" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>428</v>
       </c>
@@ -32083,10 +33058,19 @@
         <v>1855</v>
       </c>
       <c r="D104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E104">
+        <v>17.310283019881499</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G104" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>422</v>
       </c>
@@ -32097,10 +33081,19 @@
         <v>1856</v>
       </c>
       <c r="D105">
-        <v>1507.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+        <v>27309</v>
+      </c>
+      <c r="E105">
+        <v>171.20549133664099</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G105" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>426</v>
       </c>
@@ -32111,10 +33104,19 @@
         <v>1857</v>
       </c>
       <c r="D106">
-        <v>14.778678213916701</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.357921999999999</v>
+      </c>
+      <c r="E106">
+        <v>8.2718038994302798</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G106" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>430</v>
       </c>
@@ -32125,10 +33127,19 @@
         <v>1858</v>
       </c>
       <c r="D107">
-        <v>191.51795764346301</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>23.563514895374201</v>
+      </c>
+      <c r="F107" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G107" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>434</v>
       </c>
@@ -32139,10 +33150,19 @@
         <v>1859</v>
       </c>
       <c r="D108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.8131750000000002</v>
+      </c>
+      <c r="E108">
+        <v>4.5103014923570299</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G108" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>440</v>
       </c>
@@ -32153,10 +33173,19 @@
         <v>1860</v>
       </c>
       <c r="D109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E109">
+        <v>19.705046151839401</v>
+      </c>
+      <c r="F109" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G109" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>442</v>
       </c>
@@ -32167,10 +33196,19 @@
         <v>1861</v>
       </c>
       <c r="D110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E110">
+        <v>6.3360080777791898</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G110" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>450</v>
       </c>
@@ -32181,10 +33219,19 @@
         <v>1862</v>
       </c>
       <c r="D111">
-        <v>3829.9778493297599</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4097.5401000000002</v>
+      </c>
+      <c r="E111">
+        <v>8.1605903199179206</v>
+      </c>
+      <c r="F111" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G111" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>454</v>
       </c>
@@ -32195,10 +33242,19 @@
         <v>1863</v>
       </c>
       <c r="D112">
-        <v>749.52749388220104</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+        <v>949.03899999999999</v>
+      </c>
+      <c r="E112">
+        <v>20.953969729969</v>
+      </c>
+      <c r="F112" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G112" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>458</v>
       </c>
@@ -32209,10 +33265,19 @@
         <v>1864</v>
       </c>
       <c r="D113">
-        <v>4.1432975981772104</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.4010730000000002</v>
+      </c>
+      <c r="E113">
+        <v>3.3786986254990499</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G113" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>462</v>
       </c>
@@ -32223,10 +33288,19 @@
         <v>1865</v>
       </c>
       <c r="D114">
-        <v>15.3726984126984</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15.386625</v>
+      </c>
+      <c r="E114">
+        <v>2.3331433762456699</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G114" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>466</v>
       </c>
@@ -32237,10 +33311,19 @@
         <v>1866</v>
       </c>
       <c r="D115">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E115">
+        <v>9.6214760848907197</v>
+      </c>
+      <c r="F115" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G115" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>470</v>
       </c>
@@ -32251,10 +33334,19 @@
         <v>1867</v>
       </c>
       <c r="D116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962400000000002</v>
+      </c>
+      <c r="E116">
+        <v>6.1537562193303703</v>
+      </c>
+      <c r="F116" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G116" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>474</v>
       </c>
@@ -32265,10 +33357,19 @@
         <v>1868</v>
       </c>
       <c r="D117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G117" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>478</v>
       </c>
@@ -32279,10 +33380,19 @@
         <v>1870</v>
       </c>
       <c r="D118">
-        <v>37.189166666666701</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36.979999999999997</v>
+      </c>
+      <c r="E118">
+        <v>9.5252662862283408</v>
+      </c>
+      <c r="F118" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G118" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>480</v>
       </c>
@@ -32293,10 +33403,19 @@
         <v>1871</v>
       </c>
       <c r="D119">
-        <v>41.692133333333302</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44.1828</v>
+      </c>
+      <c r="E119">
+        <v>10.7737512242898</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G119" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>175</v>
       </c>
@@ -32307,10 +33426,19 @@
         <v>1872</v>
       </c>
       <c r="D120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G120" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>484</v>
       </c>
@@ -32321,10 +33449,19 @@
         <v>1874</v>
       </c>
       <c r="D121">
-        <v>20.272408333333299</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20.12735</v>
+      </c>
+      <c r="E121">
+        <v>7.8962761916854998</v>
+      </c>
+      <c r="F121" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G121" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>583</v>
       </c>
@@ -32337,8 +33474,17 @@
       <c r="D122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E122">
+        <v>5.4087437547906703</v>
+      </c>
+      <c r="F122" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G122" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>496</v>
       </c>
@@ -32349,10 +33495,19 @@
         <v>1877</v>
       </c>
       <c r="D123">
-        <v>2849.2886145414</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3140.6779000000001</v>
+      </c>
+      <c r="E123">
+        <v>15.1479560897226</v>
+      </c>
+      <c r="F123" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G123" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>499</v>
       </c>
@@ -32363,10 +33518,19 @@
         <v>1878</v>
       </c>
       <c r="D124">
-        <v>0.84537656436794495</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.95091599999999998</v>
+      </c>
+      <c r="E124">
+        <v>13.0403036347004</v>
+      </c>
+      <c r="F124" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G124" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>504</v>
       </c>
@@ -32377,10 +33541,19 @@
         <v>1879</v>
       </c>
       <c r="D125">
-        <v>8.9884840241413801</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10.16066</v>
+      </c>
+      <c r="E125">
+        <v>6.6570420275906699</v>
+      </c>
+      <c r="F125" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G125" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>508</v>
       </c>
@@ -32391,10 +33564,19 @@
         <v>1880</v>
       </c>
       <c r="D126">
-        <v>65.465000000000003</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63.850833000000002</v>
+      </c>
+      <c r="E126">
+        <v>10.279401809342099</v>
+      </c>
+      <c r="F126" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G126" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>104</v>
       </c>
@@ -32405,10 +33587,19 @@
         <v>1881</v>
       </c>
       <c r="D127">
-        <v>1381.61916666667</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2013.0416666666999</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G127" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>516</v>
       </c>
@@ -32419,10 +33610,19 @@
         <v>1882</v>
       </c>
       <c r="D128">
-        <v>14.778675</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.355858000000001</v>
+      </c>
+      <c r="E128">
+        <v>6.0812811411241299</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G128" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>524</v>
       </c>
@@ -32433,10 +33633,19 @@
         <v>1883</v>
       </c>
       <c r="D129">
-        <v>118.134081604947</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+        <v>120.84027376</v>
+      </c>
+      <c r="E129">
+        <v>7.6507917679853001</v>
+      </c>
+      <c r="F129" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G129" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>528</v>
       </c>
@@ -32447,10 +33656,19 @@
         <v>1884</v>
       </c>
       <c r="D130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E130">
+        <v>10.001207875347299</v>
+      </c>
+      <c r="F130" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G130" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>540</v>
       </c>
@@ -32461,10 +33679,19 @@
         <v>1885</v>
       </c>
       <c r="D131">
-        <v>100.88022256618601</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+        <v>113.474367</v>
+      </c>
+      <c r="E131">
+        <v>0.57831743552075399</v>
+      </c>
+      <c r="F131" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G131" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>554</v>
       </c>
@@ -32475,10 +33702,19 @@
         <v>1886</v>
       </c>
       <c r="D132">
-        <v>1.4137999999999999</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.5771833333333301</v>
+      </c>
+      <c r="E132">
+        <v>7.1722247601644096</v>
+      </c>
+      <c r="F132" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G132" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>558</v>
       </c>
@@ -32489,10 +33725,19 @@
         <v>1887</v>
       </c>
       <c r="D133">
-        <v>35.171016666666702</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35.874420999999998</v>
+      </c>
+      <c r="E133">
+        <v>10.4674244465991</v>
+      </c>
+      <c r="F133" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G133" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>562</v>
       </c>
@@ -32503,10 +33748,19 @@
         <v>1888</v>
       </c>
       <c r="D134">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E134">
+        <v>4.22621791916393</v>
+      </c>
+      <c r="F134" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G134" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>566</v>
       </c>
@@ -32517,10 +33771,19 @@
         <v>1889</v>
       </c>
       <c r="D135">
-        <v>358.81079725829699</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+        <v>428.17286256789998</v>
+      </c>
+      <c r="E135">
+        <v>18.847187784327399</v>
+      </c>
+      <c r="F135" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G135" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>578</v>
       </c>
@@ -32531,10 +33794,19 @@
         <v>1890</v>
       </c>
       <c r="D136">
-        <v>8.59</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.6141666666666694</v>
+      </c>
+      <c r="E136">
+        <v>5.7641231785227198</v>
+      </c>
+      <c r="F136" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G136" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>275</v>
       </c>
@@ -32547,8 +33819,17 @@
       <c r="D137">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G137" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>512</v>
       </c>
@@ -32561,8 +33842,17 @@
       <c r="D138">
         <v>0.38450000000000001</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E138">
+        <v>2.8118409747716302</v>
+      </c>
+      <c r="F138" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G138" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>586</v>
       </c>
@@ -32573,10 +33863,19 @@
         <v>1893</v>
       </c>
       <c r="D139">
-        <v>162.90625374741799</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+        <v>177.806331</v>
+      </c>
+      <c r="E139">
+        <v>19.873859964665499</v>
+      </c>
+      <c r="F139" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G139" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>591</v>
       </c>
@@ -32589,8 +33888,17 @@
       <c r="D140">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E140">
+        <v>2.8574828218532802</v>
+      </c>
+      <c r="F140" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G140" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>598</v>
       </c>
@@ -32601,10 +33909,19 @@
         <v>1895</v>
       </c>
       <c r="D141">
-        <v>3.5087719298245599</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.5198870000000002</v>
+      </c>
+      <c r="E141">
+        <v>5.25323922215241</v>
+      </c>
+      <c r="F141" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G141" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>600</v>
       </c>
@@ -32615,10 +33932,19 @@
         <v>1896</v>
       </c>
       <c r="D142">
-        <v>6774.1627348484899</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6982.7524000000003</v>
+      </c>
+      <c r="E142">
+        <v>9.7655666716440201</v>
+      </c>
+      <c r="F142" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G142" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>604</v>
       </c>
@@ -32629,10 +33955,19 @@
         <v>1897</v>
       </c>
       <c r="D143">
-        <v>3.8805541313758698</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.835181</v>
+      </c>
+      <c r="E143">
+        <v>8.3337063009623105</v>
+      </c>
+      <c r="F143" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G143" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>608</v>
       </c>
@@ -32643,10 +33978,19 @@
         <v>1898</v>
       </c>
       <c r="D144">
-        <v>49.254597728841198</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54.477786000000002</v>
+      </c>
+      <c r="E144">
+        <v>5.8211581121395497</v>
+      </c>
+      <c r="F144" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G144" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>616</v>
       </c>
@@ -32657,10 +34001,19 @@
         <v>1899</v>
       </c>
       <c r="D145">
-        <v>3.8619166666666702</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.4577583333000002</v>
+      </c>
+      <c r="E145">
+        <v>14.4294507575758</v>
+      </c>
+      <c r="F145" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G145" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>620</v>
       </c>
@@ -32671,10 +34024,19 @@
         <v>1900</v>
       </c>
       <c r="D146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E146">
+        <v>7.8326912423332304</v>
+      </c>
+      <c r="F146" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G146" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>630</v>
       </c>
@@ -32687,8 +34049,17 @@
       <c r="D147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G147" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>634</v>
       </c>
@@ -32701,8 +34072,17 @@
       <c r="D148">
         <v>3.64</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E148">
+        <v>4.9952755374076103</v>
+      </c>
+      <c r="F148" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G148" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>410</v>
       </c>
@@ -32713,10 +34093,19 @@
         <v>1903</v>
       </c>
       <c r="D149">
-        <v>1143.95166666667</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1291.4467</v>
+      </c>
+      <c r="E149">
+        <v>5.0878876079284803</v>
+      </c>
+      <c r="F149" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G149" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>498</v>
       </c>
@@ -32727,10 +34116,19 @@
         <v>1904</v>
       </c>
       <c r="D150">
-        <v>17.680466141833101</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E150">
+        <v>28.737297676623498</v>
+      </c>
+      <c r="F150" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G150" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>638</v>
       </c>
@@ -32743,8 +34141,17 @@
       <c r="D151">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G151" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>642</v>
       </c>
@@ -32755,10 +34162,19 @@
         <v>1907</v>
       </c>
       <c r="D152">
-        <v>4.16041666666667</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.6884750000000004</v>
+      </c>
+      <c r="E152">
+        <v>13.795488743252101</v>
+      </c>
+      <c r="F152" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G152" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>643</v>
       </c>
@@ -32769,10 +34185,19 @@
         <v>1908</v>
       </c>
       <c r="D153">
-        <v>73.654349999999994</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+        <v>68.484942000000004</v>
+      </c>
+      <c r="E153">
+        <v>6.6944589195763697</v>
+      </c>
+      <c r="F153" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G153" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>646</v>
       </c>
@@ -32783,10 +34208,19 @@
         <v>1909</v>
       </c>
       <c r="D154">
-        <v>988.62480655176796</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1030.3082999999999</v>
+      </c>
+      <c r="E154">
+        <v>17.689209558815399</v>
+      </c>
+      <c r="F154" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G154" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>659</v>
       </c>
@@ -32799,8 +34233,17 @@
       <c r="D155">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E155">
+        <v>2.6673884269324302</v>
+      </c>
+      <c r="F155" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G155" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>662</v>
       </c>
@@ -32813,8 +34256,17 @@
       <c r="D156">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E156">
+        <v>6.3781469513337203</v>
+      </c>
+      <c r="F156" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G156" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>670</v>
       </c>
@@ -32827,8 +34279,17 @@
       <c r="D157">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E157">
+        <v>5.6600977922658</v>
+      </c>
+      <c r="F157" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G157" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>882</v>
       </c>
@@ -32839,10 +34300,19 @@
         <v>1913</v>
       </c>
       <c r="D158">
-        <v>2.5560923420784398</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.6054140000000001</v>
+      </c>
+      <c r="E158">
+        <v>10.9618822286844</v>
+      </c>
+      <c r="F158" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G158" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>5733</v>
       </c>
@@ -32850,13 +34320,22 @@
         <v>1914</v>
       </c>
       <c r="C159" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="D159">
         <v>100</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G159" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>678</v>
       </c>
@@ -32867,10 +34346,19 @@
         <v>1915</v>
       </c>
       <c r="D160">
-        <v>21.507059099358202</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23.465267000000001</v>
+      </c>
+      <c r="E160">
+        <v>18.005635112284601</v>
+      </c>
+      <c r="F160" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G160" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>682</v>
       </c>
@@ -32883,8 +34371,17 @@
       <c r="D161">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E161">
+        <v>2.4740737192536999</v>
+      </c>
+      <c r="F161" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G161" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>686</v>
       </c>
@@ -32895,10 +34392,19 @@
         <v>1917</v>
       </c>
       <c r="D162">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E162">
+        <v>9.6968189908107298</v>
+      </c>
+      <c r="F162" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G162" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>688</v>
       </c>
@@ -32909,10 +34415,19 @@
         <v>1918</v>
       </c>
       <c r="D163">
-        <v>99.395941666666701</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111.6622</v>
+      </c>
+      <c r="E163">
+        <v>11.981511734470301</v>
+      </c>
+      <c r="F163" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G163" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>690</v>
       </c>
@@ -32923,10 +34438,19 @@
         <v>1919</v>
       </c>
       <c r="D164">
-        <v>16.9205225709613</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14.27251</v>
+      </c>
+      <c r="E164">
+        <v>8.2768581143721605</v>
+      </c>
+      <c r="F164" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G164" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>694</v>
       </c>
@@ -32937,10 +34461,19 @@
         <v>1920</v>
       </c>
       <c r="D165">
-        <v>10439.425330423601</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14.047650000000001</v>
+      </c>
+      <c r="E165">
+        <v>27.208288381465302</v>
+      </c>
+      <c r="F165" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G165" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>702</v>
       </c>
@@ -32951,10 +34484,19 @@
         <v>1921</v>
       </c>
       <c r="D166">
-        <v>1.34348333333333</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.3786670000000001</v>
+      </c>
+      <c r="E166">
+        <v>6.1210600403941804</v>
+      </c>
+      <c r="F166" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G166" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>703</v>
       </c>
@@ -32965,10 +34507,19 @@
         <v>1922</v>
       </c>
       <c r="D167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E167">
+        <v>12.774146363761099</v>
+      </c>
+      <c r="F167" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G167" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>705</v>
       </c>
@@ -32979,10 +34530,19 @@
         <v>1923</v>
       </c>
       <c r="D168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E168">
+        <v>8.8336988674945207</v>
+      </c>
+      <c r="F168" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G168" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>90</v>
       </c>
@@ -32993,10 +34553,19 @@
         <v>1924</v>
       </c>
       <c r="D169">
-        <v>8.0301029910493202</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8.1555</v>
+      </c>
+      <c r="E169">
+        <v>5.5181292857696098</v>
+      </c>
+      <c r="F169" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G169" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>706</v>
       </c>
@@ -33007,10 +34576,19 @@
         <v>1925</v>
       </c>
       <c r="D170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26832.519691000001</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G170" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>710</v>
       </c>
@@ -33021,10 +34599,19 @@
         <v>1926</v>
       </c>
       <c r="D171">
-        <v>14.778678213916701</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.355853</v>
+      </c>
+      <c r="E171">
+        <v>7.0397266125586597</v>
+      </c>
+      <c r="F171" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G171" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>728</v>
       </c>
@@ -33035,10 +34622,19 @@
         <v>1927</v>
       </c>
       <c r="D172">
-        <v>306.35461993727603</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+        <v>422.49339386999998</v>
+      </c>
+      <c r="E172">
+        <v>-6.6873209421265196</v>
+      </c>
+      <c r="F172" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G172" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>724</v>
       </c>
@@ -33049,10 +34645,19 @@
         <v>1928</v>
       </c>
       <c r="D173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.94962375315694103</v>
+      </c>
+      <c r="E173">
+        <v>8.3905763411862697</v>
+      </c>
+      <c r="F173" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G173" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>144</v>
       </c>
@@ -33063,10 +34668,19 @@
         <v>1929</v>
       </c>
       <c r="D174">
-        <v>185.59255777221301</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+        <v>324.55059999999997</v>
+      </c>
+      <c r="E174">
+        <v>49.721102111433098</v>
+      </c>
+      <c r="F174" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G174" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>729</v>
       </c>
@@ -33077,10 +34691,19 @@
         <v>1930</v>
       </c>
       <c r="D175">
-        <v>53.9960119047619</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+        <v>556.6</v>
+      </c>
+      <c r="E175">
+        <v>138.80846024176</v>
+      </c>
+      <c r="F175" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G175" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>740</v>
       </c>
@@ -33091,10 +34714,19 @@
         <v>1931</v>
       </c>
       <c r="D176">
-        <v>18.238666666666699</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+        <v>24.709174999999998</v>
+      </c>
+      <c r="E176">
+        <v>52.446027276240798</v>
+      </c>
+      <c r="F176" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G176" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>748</v>
       </c>
@@ -33105,10 +34737,19 @@
         <v>1932</v>
       </c>
       <c r="D177">
-        <v>14.783435139578399</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.362283000000001</v>
+      </c>
+      <c r="E177">
+        <v>2.5980162031107699</v>
+      </c>
+      <c r="F177" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G177" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>752</v>
       </c>
@@ -33119,10 +34760,19 @@
         <v>1933</v>
       </c>
       <c r="D178">
-        <v>8.5765667160737795</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10.114251277564</v>
+      </c>
+      <c r="E178">
+        <v>8.3692909886918905</v>
+      </c>
+      <c r="F178" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G178" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>756</v>
       </c>
@@ -33133,10 +34783,19 @@
         <v>1934</v>
       </c>
       <c r="D179">
-        <v>0.91384583333333302</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.95483249999999997</v>
+      </c>
+      <c r="E179">
+        <v>2.8350279864446302</v>
+      </c>
+      <c r="F179" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G179" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>760</v>
       </c>
@@ -33147,10 +34806,19 @@
         <v>1935</v>
       </c>
       <c r="D180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3804.7807499999999</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G180" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>762</v>
       </c>
@@ -33161,10 +34829,19 @@
         <v>1936</v>
       </c>
       <c r="D181">
-        <v>11.30885</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11.031075</v>
+      </c>
+      <c r="E181">
+        <v>6.0045808232213904</v>
+      </c>
+      <c r="F181" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G181" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>807</v>
       </c>
@@ -33175,10 +34852,19 @@
         <v>1937</v>
       </c>
       <c r="D182">
-        <v>52.1021583333333</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58.599902</v>
+      </c>
+      <c r="E182">
+        <v>14.204717319583301</v>
+      </c>
+      <c r="F182" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G182" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>764</v>
       </c>
@@ -33189,10 +34875,19 @@
         <v>1938</v>
       </c>
       <c r="D183">
-        <v>31.9770934417717</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35.061399999999999</v>
+      </c>
+      <c r="E183">
+        <v>6.0774122843431897</v>
+      </c>
+      <c r="F183" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G183" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>626</v>
       </c>
@@ -33205,8 +34900,17 @@
       <c r="D184">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E184">
+        <v>0.958812739702808</v>
+      </c>
+      <c r="F184" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G184" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>768</v>
       </c>
@@ -33217,10 +34921,19 @@
         <v>1940</v>
       </c>
       <c r="D185">
-        <v>554.53067503310399</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+        <v>623.75970099999995</v>
+      </c>
+      <c r="E185">
+        <v>7.96757361617885</v>
+      </c>
+      <c r="F185" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G185" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>776</v>
       </c>
@@ -33231,10 +34944,19 @@
         <v>1941</v>
       </c>
       <c r="D186">
-        <v>2.2649596005005499</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.2717510000000001</v>
+      </c>
+      <c r="E186">
+        <v>10.971365290302201</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G186" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>780</v>
       </c>
@@ -33245,10 +34967,19 @@
         <v>1942</v>
       </c>
       <c r="D187">
-        <v>6.7585300491629399</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.7541000000000002</v>
+      </c>
+      <c r="E187">
+        <v>5.8283863851795896</v>
+      </c>
+      <c r="F187" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G187" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>788</v>
       </c>
@@ -33259,10 +34990,19 @@
         <v>1943</v>
       </c>
       <c r="D188">
-        <v>2.7944666666666702</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.1049000000000002</v>
+      </c>
+      <c r="E188">
+        <v>8.30646124447623</v>
+      </c>
+      <c r="F188" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G188" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>792</v>
       </c>
@@ -33273,10 +35013,19 @@
         <v>1944</v>
       </c>
       <c r="D189">
-        <v>8.8504075492831493</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.548860000000001</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G189" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>795</v>
       </c>
@@ -33287,10 +35036,19 @@
         <v>1945</v>
       </c>
       <c r="D190">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.5</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G190" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>800</v>
       </c>
@@ -33301,10 +35059,19 @@
         <v>1946</v>
       </c>
       <c r="D191">
-        <v>3587.0517073390802</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3571.6386710000002</v>
+      </c>
+      <c r="E191">
+        <v>7.1957888597580997</v>
+      </c>
+      <c r="F191" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G191" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>804</v>
       </c>
@@ -33315,10 +35082,19 @@
         <v>1947</v>
       </c>
       <c r="D192">
-        <v>27.286189383333301</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32.342301999999997</v>
+      </c>
+      <c r="E192">
+        <v>20.183636661747801</v>
+      </c>
+      <c r="F192" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G192" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>784</v>
       </c>
@@ -33331,8 +35107,17 @@
       <c r="D193">
         <v>3.6724999999999999</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E193">
+        <v>4.8278885959447502</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G193" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>826</v>
       </c>
@@ -33343,10 +35128,19 @@
         <v>1949</v>
       </c>
       <c r="D194">
-        <v>0.72706494468832195</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.811301715827773</v>
+      </c>
+      <c r="E194">
+        <v>7.9220488314790201</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G194" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>834</v>
       </c>
@@ -33357,10 +35151,19 @@
         <v>1950</v>
       </c>
       <c r="D195">
-        <v>2297.76422623792</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2302.3998580000002</v>
+      </c>
+      <c r="E195">
+        <v>4.3502720426910102</v>
+      </c>
+      <c r="F195" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G195" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>840</v>
       </c>
@@ -33373,8 +35176,17 @@
       <c r="D196">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E196">
+        <v>3</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G196" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>850</v>
       </c>
@@ -33387,8 +35199,17 @@
       <c r="D197">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G197" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>858</v>
       </c>
@@ -33399,10 +35220,19 @@
         <v>1954</v>
       </c>
       <c r="D198">
-        <v>43.554575</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41.1676</v>
+      </c>
+      <c r="E198">
+        <v>9.10437983075437</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G198" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>860</v>
       </c>
@@ -33413,10 +35243,19 @@
         <v>1955</v>
       </c>
       <c r="D199">
-        <v>10609.464390809</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11050.145422</v>
+      </c>
+      <c r="E199">
+        <v>11.446643699883399</v>
+      </c>
+      <c r="F199" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G199" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>548</v>
       </c>
@@ -33427,10 +35266,19 @@
         <v>1956</v>
       </c>
       <c r="D200">
-        <v>109.4525</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+        <v>115.3539</v>
+      </c>
+      <c r="E200">
+        <v>7.1022312964853098</v>
+      </c>
+      <c r="F200" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G200" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>862</v>
       </c>
@@ -33441,10 +35289,19 @@
         <v>1957</v>
       </c>
       <c r="D201">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>121.73808529750301</v>
+      </c>
+      <c r="F201" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G201" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>704</v>
       </c>
@@ -33455,10 +35312,19 @@
         <v>1958</v>
       </c>
       <c r="D202">
-        <v>23159.782592592601</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23271.212500000001</v>
+      </c>
+      <c r="E202">
+        <v>3.1565074996312901</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G202" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>732</v>
       </c>
@@ -33471,8 +35337,17 @@
       <c r="D203">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G203" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>887</v>
       </c>
@@ -33483,10 +35358,19 @@
         <v>1961</v>
       </c>
       <c r="D204">
-        <v>1035.4671855588699</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1114.292841</v>
+      </c>
+      <c r="E204">
+        <v>8.1047258362391492</v>
+      </c>
+      <c r="F204" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G204" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>894</v>
       </c>
@@ -33497,10 +35381,19 @@
         <v>1962</v>
       </c>
       <c r="D205">
-        <v>20.018486585968802</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.937594000000001</v>
+      </c>
+      <c r="E205">
+        <v>10.9932039209135</v>
+      </c>
+      <c r="F205" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G205" s="3">
+        <v>45379</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>716</v>
       </c>
@@ -33511,7 +35404,16 @@
         <v>1963</v>
       </c>
       <c r="D206">
-        <v>88.552447259743602</v>
+        <v>452.68413099999998</v>
+      </c>
+      <c r="E206">
+        <v>104.70517062866701</v>
+      </c>
+      <c r="F206" t="s">
+        <v>1969</v>
+      </c>
+      <c r="G206" s="3">
+        <v>45379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed inflation for U.S.
</commit_message>
<xml_diff>
--- a/SourceData/ohtcore/IHModData.xlsx
+++ b/SourceData/ohtcore/IHModData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\ohtcore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF13D078-470C-4B7E-B331-99041193B3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6D130B-C0F1-4C72-8702-ABD133633D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CommentsOutline" sheetId="2" r:id="rId1"/>
@@ -6007,28 +6007,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7E262D65-9DFC-4FE9-9672-D6D67E4FBFAB}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -30680,8 +30659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D8DDA6-9117-4ADB-B296-670BDA511577}">
   <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="I190" sqref="I190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35177,7 +35156,7 @@
         <v>1</v>
       </c>
       <c r="E196">
-        <v>3</v>
+        <v>8.0027998205212096</v>
       </c>
       <c r="F196" t="s">
         <v>1969</v>

</xml_diff>